<commit_message>
Update in ml code
</commit_message>
<xml_diff>
--- a/Project/dataset.xlsx
+++ b/Project/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7746d68f5b450d6f/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\chatbot_aiml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2142D00-9C9F-48D6-BCFF-7317B136B4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91D99A5-22D8-4882-B8C2-EDFA3056BBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3780C01F-CE97-4B9B-8BBA-01EE4026DA53}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Query ID</t>
   </si>
@@ -47,113 +47,104 @@
     <t>Intent Label</t>
   </si>
   <si>
-    <t>Additional Context</t>
-  </si>
-  <si>
     <t>When are the final exams scheduled?</t>
   </si>
   <si>
     <t>Exam Schedule</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>What are the course details for ECE 101?</t>
   </si>
   <si>
     <t>Course Details</t>
   </si>
   <si>
-    <t>Course Code: ECE 101</t>
-  </si>
-  <si>
-    <t>Course Code: ECE 102</t>
-  </si>
-  <si>
     <t>How can I access my previous semester results?</t>
   </si>
   <si>
     <t>Grade Inquiry</t>
   </si>
   <si>
-    <t>Previous Semester</t>
-  </si>
-  <si>
     <t>Where can I find the library hours?</t>
   </si>
   <si>
     <t>General Inquiry</t>
   </si>
   <si>
-    <t>Facility: Library</t>
-  </si>
-  <si>
     <t>What is the prerequisite for ECE 202?</t>
   </si>
   <si>
     <t>Prerequisites</t>
   </si>
   <si>
-    <t>Course Code: ECE 202</t>
-  </si>
-  <si>
-    <t>Course Code: ECE 203</t>
-  </si>
-  <si>
     <t>Who is the instructor for CS101?</t>
   </si>
   <si>
     <t>Instructor Info</t>
   </si>
   <si>
-    <t>Course Code: CS101</t>
-  </si>
-  <si>
-    <t>Course Code: CS102</t>
-  </si>
-  <si>
     <t>Can I change my major?</t>
   </si>
   <si>
     <t>Academic Policies</t>
   </si>
   <si>
-    <t>Major Change</t>
-  </si>
-  <si>
     <t>When do classes start for the next semester?</t>
   </si>
   <si>
     <t>Academic Calendar</t>
   </si>
   <si>
-    <t>Next Semester</t>
-  </si>
-  <si>
     <t>How do I apply for graduation?</t>
   </si>
   <si>
     <t>Graduation Process</t>
   </si>
   <si>
-    <t>Application Process</t>
-  </si>
-  <si>
     <t>How can I join a student club?</t>
   </si>
   <si>
     <t>Extracurricular</t>
   </si>
   <si>
-    <t>Club Joining</t>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Final exams are scheduled from December 10th to December 20th.</t>
+  </si>
+  <si>
+    <t>ECE 101 is an introductory course on electronics. It covers basic circuit theory and electronic devices. Instructor: Prof. Srinivasa Rao.</t>
+  </si>
+  <si>
+    <t>You can access your previous semester results via the student portal under the "Grades" section.</t>
+  </si>
+  <si>
+    <t>The library is open from 8 AM to 9 PM on weekdays, and from 10 AM to 2 PM on weekends.</t>
+  </si>
+  <si>
+    <t>The prerequisite for ECE 202 is ECE 101.</t>
+  </si>
+  <si>
+    <t>The instructor for CS101 is Dr. Priya Mehta.</t>
+  </si>
+  <si>
+    <t>Yes, you can change your major by submitting a request to the academic office. The deadline for major change requests is November 15th.</t>
+  </si>
+  <si>
+    <t>Classes for the next semester start on January 5th.</t>
+  </si>
+  <si>
+    <t>You can apply for graduation by filling out the graduation application form on the student portal. The deadline for applications is April 1st.</t>
+  </si>
+  <si>
+    <t>You can join a student club by attending the club fairs held at the start of each semester or by contacting the club coordinators directly.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,9 +213,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -262,7 +253,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -368,7 +359,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -510,7 +501,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -520,20 +511,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9135F1C4-2886-4B6F-BDED-4BCF848FF960}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,181 +535,159 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="87">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="87">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="87">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="72.599999999999994">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="72.599999999999994">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="72.599999999999994">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="57.95">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="87">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="57.95">
+        <v>31</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="57.95">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E11" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Update in forntend and ml logic
</commit_message>
<xml_diff>
--- a/Project/dataset.xlsx
+++ b/Project/dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\chatbot_aiml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\AIML_Project\AIML-PROJECT-2320040080\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91D99A5-22D8-4882-B8C2-EDFA3056BBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D223B4CD-E6CA-4D58-AF9B-18E73159F1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3780C01F-CE97-4B9B-8BBA-01EE4026DA53}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>